<commit_message>
new branch created. training loss over time (cost vs iteration) addd as output plot. looking for smooth decline without oscillations.
</commit_message>
<xml_diff>
--- a/Batch_Optimization.xlsx
+++ b/Batch_Optimization.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derrick.magdefrau\Documents\GitHub\Masters_Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derrick\Documents\GitHub\Masters_Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2671AA5-9FF4-4F55-B862-94C17D97E34E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E141A2-F13F-4C91-818C-5DCD2169CF06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="5136" xr2:uid="{E305303A-8BBB-401C-B59B-0762E69B7640}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12285" windowHeight="5130" activeTab="1" xr2:uid="{E305303A-8BBB-401C-B59B-0762E69B7640}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Normal" sheetId="2" r:id="rId1"/>
+    <sheet name="Oversampled" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="42">
   <si>
     <t>n_folds</t>
   </si>
@@ -128,14 +129,41 @@
     <t>Trial 12</t>
   </si>
   <si>
-    <t>Trial 13</t>
+    <t>Trial 14</t>
+  </si>
+  <si>
+    <t>Trial 15</t>
+  </si>
+  <si>
+    <t>Trial 16</t>
+  </si>
+  <si>
+    <t>Trial 17</t>
+  </si>
+  <si>
+    <t>Trial 18</t>
+  </si>
+  <si>
+    <t>Trial 19</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>Trial 20</t>
+  </si>
+  <si>
+    <t>Trial 21</t>
+  </si>
+  <si>
+    <t>Trial 22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,13 +171,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,12 +206,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -194,13 +249,282 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3727450</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F24E11-E070-4B54-988D-118AECCDB562}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2295525" y="4219575"/>
+          <a:ext cx="3632200" cy="2724150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3714750</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB7FD0F1-7FBF-4000-8123-0C3C6FACC446}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2276475" y="7239000"/>
+          <a:ext cx="3638550" cy="2728913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3746500</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30797492-824B-416C-A928-2D4162B56029}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2238375" y="10125075"/>
+          <a:ext cx="3708400" cy="2781300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3717925</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DDCF4D2-A0CD-42BA-8D25-834A564FD461}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="36318825" y="4210050"/>
+          <a:ext cx="3632200" cy="2724150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3759200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23B29989-0A8B-4B23-BD94-4E64275F2155}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="36271200" y="7286625"/>
+          <a:ext cx="3721100" cy="2790825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3752850</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1D39849-9F21-40CC-94F5-4E30CAC71D5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="36290250" y="10325100"/>
+          <a:ext cx="3695700" cy="2771775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>3886201</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>144781</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3867512</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>362</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>135256</xdr:rowOff>
     </xdr:to>
@@ -244,7 +568,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3864962</xdr:colOff>
+      <xdr:colOff>3779237</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -287,8 +611,8 @@
       <xdr:rowOff>144781</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3867512</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>362</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>135256</xdr:rowOff>
     </xdr:to>
@@ -332,7 +656,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3864990</xdr:colOff>
+      <xdr:colOff>3779265</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>129541</xdr:rowOff>
     </xdr:to>
@@ -375,8 +699,8 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3867512</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>362</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -420,7 +744,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3863730</xdr:colOff>
+      <xdr:colOff>3778005</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>135255</xdr:rowOff>
     </xdr:to>
@@ -463,8 +787,8 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3867512</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>362</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -508,7 +832,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3828795</xdr:colOff>
+      <xdr:colOff>3781170</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>154306</xdr:rowOff>
     </xdr:to>
@@ -551,8 +875,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3886534</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>334</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>131445</xdr:rowOff>
     </xdr:to>
@@ -595,8 +919,8 @@
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3869417</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2267</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>167641</xdr:rowOff>
     </xdr:to>
@@ -640,7 +964,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3882724</xdr:colOff>
+      <xdr:colOff>3777949</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>59055</xdr:rowOff>
     </xdr:to>
@@ -684,7 +1008,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3845295</xdr:colOff>
+      <xdr:colOff>3778620</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -727,8 +1051,8 @@
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3888467</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2267</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
@@ -771,8 +1095,8 @@
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3848100</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>53436</xdr:rowOff>
     </xdr:to>
@@ -816,7 +1140,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3825719</xdr:colOff>
+      <xdr:colOff>3778094</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
@@ -859,8 +1183,8 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>3870060</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2910</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
@@ -904,7 +1228,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3863702</xdr:colOff>
+      <xdr:colOff>3777977</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
@@ -947,8 +1271,8 @@
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>3867151</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>56388</xdr:rowOff>
     </xdr:to>
@@ -992,7 +1316,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3845323</xdr:colOff>
+      <xdr:colOff>3778648</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>74296</xdr:rowOff>
     </xdr:to>
@@ -1035,8 +1359,8 @@
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>3867540</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1080,7 +1404,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3864345</xdr:colOff>
+      <xdr:colOff>3778620</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
@@ -1123,8 +1447,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3850395</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2295</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
@@ -1168,7 +1492,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>3864345</xdr:colOff>
+      <xdr:colOff>3778620</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
@@ -1212,7 +1536,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>3828178</xdr:colOff>
+      <xdr:colOff>3780553</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
@@ -1255,8 +1579,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3868155</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1005</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>59055</xdr:rowOff>
     </xdr:to>
@@ -1300,7 +1624,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>3789825</xdr:colOff>
+      <xdr:colOff>3780300</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>93345</xdr:rowOff>
     </xdr:to>
@@ -1343,8 +1667,8 @@
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3830083</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1033</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>17146</xdr:rowOff>
     </xdr:to>
@@ -1387,8 +1711,8 @@
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3868800</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1650</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>59056</xdr:rowOff>
     </xdr:to>
@@ -1431,8 +1755,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3848573</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>473</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>173355</xdr:rowOff>
     </xdr:to>
@@ -1476,7 +1800,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3866895</xdr:colOff>
+      <xdr:colOff>3781170</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>59056</xdr:rowOff>
     </xdr:to>
@@ -1520,7 +1844,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>3788201</xdr:colOff>
+      <xdr:colOff>3778676</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -1564,7 +1888,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>3825630</xdr:colOff>
+      <xdr:colOff>3778005</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -1608,7 +1932,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>3807251</xdr:colOff>
+      <xdr:colOff>3778676</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
@@ -1651,8 +1975,8 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>3793916</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2966</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1696,7 +2020,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>3825658</xdr:colOff>
+      <xdr:colOff>3778033</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>91441</xdr:rowOff>
     </xdr:to>
@@ -1740,7 +2064,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>3807223</xdr:colOff>
+      <xdr:colOff>3778648</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>135256</xdr:rowOff>
     </xdr:to>
@@ -1784,7 +2108,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>3883367</xdr:colOff>
+      <xdr:colOff>3778592</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
@@ -1828,7 +2152,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>3828795</xdr:colOff>
+      <xdr:colOff>3781170</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
@@ -1866,13 +2190,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>3868155</xdr:colOff>
+      <xdr:colOff>3763380</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>173355</xdr:rowOff>
     </xdr:to>
@@ -1899,6 +2223,666 @@
         <a:xfrm>
           <a:off x="49034700" y="7067550"/>
           <a:ext cx="3845295" cy="2882265"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3724275</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>126206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BF9C297-0019-45E2-9015-90ADB77D8C0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="55140225" y="4191000"/>
+          <a:ext cx="3724275" cy="2793206"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3724275</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>126207</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA95C3B5-D188-4A90-8497-D4449322559A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="55140225" y="7239001"/>
+          <a:ext cx="3724275" cy="2793206"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>3702050</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AE9732C-6869-47BF-A83F-E3CD3273A342}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="55197375" y="10287000"/>
+          <a:ext cx="3644900" cy="2733675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3676650</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08FF2B32-6813-4638-B3A5-137EBFFC5EF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="55159275" y="4114800"/>
+          <a:ext cx="3657600" cy="2743200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3746499</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0014248-8003-4806-B608-E37180F4CF1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="55206899" y="7248525"/>
+          <a:ext cx="3679825" cy="2809875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3724275</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF6A00D3-D655-4352-9D70-DFCC0D4A1BBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="55168800" y="10201275"/>
+          <a:ext cx="3695700" cy="2771775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>3756025</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C50BE30-E362-4A6C-9596-153E02179427}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="58969275" y="4048125"/>
+          <a:ext cx="3708400" cy="2781300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>3749675</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C99497B-AC4A-4AD8-9B33-6361D6E91BA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="58950225" y="7048500"/>
+          <a:ext cx="3721100" cy="2790825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>3733800</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C45023B2-BF4A-4902-9FE8-5348FB0EBD68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="58997850" y="10096500"/>
+          <a:ext cx="3657600" cy="2743200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>3692525</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9BF0812-D685-4607-998E-3BD85F457C3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="62788800" y="4067175"/>
+          <a:ext cx="3606800" cy="2705100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>3746500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74E88107-6509-4045-BB96-033BB7184DB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="62741175" y="7010400"/>
+          <a:ext cx="3708400" cy="2781300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>3736975</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F21B55-40D1-4CF2-847C-38413300AFA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="62731650" y="10086975"/>
+          <a:ext cx="3708400" cy="2781300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>3667125</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C65F472B-30A3-4FF8-9587-BF78535AC848}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66551175" y="4086225"/>
+          <a:ext cx="3600450" cy="2700338"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>3724275</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8CB3D64-7EFC-4FEE-AE82-95B0786588BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66560700" y="7038975"/>
+          <a:ext cx="3648075" cy="2736056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>3743325</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F0890AE-CBF2-41B1-843E-3E3BC3D9E550}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66513075" y="10096500"/>
+          <a:ext cx="3714750" cy="2786063"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2206,62 +3190,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2357D04-C28B-44E3-B5FB-928058F75E94}">
-  <dimension ref="A2:N21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49489416-574D-473C-A336-82E57285D721}">
+  <dimension ref="A2:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K7" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="14" width="56.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="19" width="56.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="O2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
@@ -2291,7 +3294,7 @@
       <c r="J3" s="1">
         <v>10</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="6">
         <v>10</v>
       </c>
       <c r="L3" s="1">
@@ -2303,9 +3306,24 @@
       <c r="N3" s="1">
         <v>10</v>
       </c>
+      <c r="O3" s="1">
+        <v>10</v>
+      </c>
+      <c r="P3" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>10</v>
+      </c>
+      <c r="R3" s="1">
+        <v>10</v>
+      </c>
+      <c r="S3" s="1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
@@ -2335,7 +3353,7 @@
       <c r="J4" s="1">
         <v>0.1</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="6">
         <v>0.1</v>
       </c>
       <c r="L4" s="1">
@@ -2347,9 +3365,24 @@
       <c r="N4" s="1">
         <v>0.1</v>
       </c>
+      <c r="O4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
@@ -2379,7 +3412,7 @@
       <c r="J5" s="1">
         <v>0.5</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="6">
         <v>0.5</v>
       </c>
       <c r="L5" s="1">
@@ -2391,9 +3424,888 @@
       <c r="N5" s="1">
         <v>0.5</v>
       </c>
+      <c r="O5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="R8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1000</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>1000</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>500</v>
+      </c>
+      <c r="C10" s="1">
+        <v>500</v>
+      </c>
+      <c r="D10" s="1">
+        <v>500</v>
+      </c>
+      <c r="E10" s="1">
+        <v>100</v>
+      </c>
+      <c r="F10" s="1">
+        <v>100</v>
+      </c>
+      <c r="G10" s="1">
+        <v>100</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K10" s="6">
+        <v>2000</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2000</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2000</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1500</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1500</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1250</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>1750</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1750</v>
+      </c>
+      <c r="S10" s="1">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1">
+        <v>10</v>
+      </c>
+      <c r="K12" s="6">
+        <v>10</v>
+      </c>
+      <c r="L12" s="1">
+        <v>10</v>
+      </c>
+      <c r="M12" s="1">
+        <v>10</v>
+      </c>
+      <c r="N12" s="1">
+        <v>10</v>
+      </c>
+      <c r="O12" s="1">
+        <v>10</v>
+      </c>
+      <c r="P12" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>10</v>
+      </c>
+      <c r="R12" s="1">
+        <v>10</v>
+      </c>
+      <c r="S12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K13" s="6"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0.96</v>
+      </c>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="6"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0.96</v>
+      </c>
+      <c r="Q16" s="6"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="Q17" s="6"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="Q18" s="6"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>58.68</v>
+      </c>
+      <c r="K19" s="6">
+        <v>35.26</v>
+      </c>
+      <c r="Q19" s="6"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K20" s="6"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" ref="B21:M21" si="0">B14/B19</f>
+        <v>1.6700749829584187E-2</v>
+      </c>
+      <c r="C21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7226318774815655E-2</v>
+      </c>
+      <c r="L21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" s="1" t="e">
+        <f>N14/N19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="1" t="e">
+        <f>O14/O19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21" s="1" t="e">
+        <f t="shared" ref="P21:Q21" si="1">P14/P19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q21" s="6" t="e">
+        <f>Q14/Q19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R21" s="1" t="e">
+        <f>R14/R19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S21" s="1" t="e">
+        <f>S14/S19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2357D04-C28B-44E3-B5FB-928058F75E94}">
+  <dimension ref="A2:V21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="T20" sqref="T20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="22" width="56.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1">
+        <v>10</v>
+      </c>
+      <c r="K3" s="6">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1">
+        <v>10</v>
+      </c>
+      <c r="M3" s="1">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1">
+        <v>10</v>
+      </c>
+      <c r="O3" s="1">
+        <v>10</v>
+      </c>
+      <c r="P3" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>10</v>
+      </c>
+      <c r="R3" s="1">
+        <v>10</v>
+      </c>
+      <c r="S3" s="1">
+        <v>10</v>
+      </c>
+      <c r="T3" s="1">
+        <v>10</v>
+      </c>
+      <c r="U3" s="1">
+        <v>10</v>
+      </c>
+      <c r="V3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2423,7 +4335,7 @@
       <c r="J6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -2435,9 +4347,33 @@
       <c r="N6" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="O6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
@@ -2467,7 +4403,7 @@
       <c r="J7" s="1">
         <v>0.5</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="6">
         <v>0.5</v>
       </c>
       <c r="L7" s="1">
@@ -2479,9 +4415,33 @@
       <c r="N7" s="1">
         <v>0.5</v>
       </c>
+      <c r="O7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1">
@@ -2511,7 +4471,7 @@
       <c r="J8" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="6">
         <v>1E-3</v>
       </c>
       <c r="L8" s="1">
@@ -2523,9 +4483,33 @@
       <c r="N8" s="1">
         <v>1E-3</v>
       </c>
+      <c r="O8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="R8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="T8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="V8" s="1">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1">
@@ -2555,7 +4539,7 @@
       <c r="J9" s="1">
         <v>1000</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="6">
         <v>1000</v>
       </c>
       <c r="L9" s="1">
@@ -2567,9 +4551,33 @@
       <c r="N9" s="1">
         <v>1000</v>
       </c>
+      <c r="O9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>1000</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="T9" s="1">
+        <v>3000</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="V9" s="1">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1">
@@ -2599,7 +4607,7 @@
       <c r="J10" s="1">
         <v>1000</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="6">
         <v>2000</v>
       </c>
       <c r="L10" s="1">
@@ -2609,11 +4617,35 @@
         <v>2000</v>
       </c>
       <c r="N10" s="1">
+        <v>1500</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1500</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1250</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>1750</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1750</v>
+      </c>
+      <c r="S10" s="1">
+        <v>1750</v>
+      </c>
+      <c r="T10" s="1">
         <v>2000</v>
       </c>
+      <c r="U10" s="1">
+        <v>2000</v>
+      </c>
+      <c r="V10" s="1">
+        <v>2000</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1">
@@ -2643,7 +4675,7 @@
       <c r="J11" s="1">
         <v>1E-4</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="6">
         <v>0.01</v>
       </c>
       <c r="L11" s="1">
@@ -2653,11 +4685,35 @@
         <v>1E-4</v>
       </c>
       <c r="N11" s="1">
-        <v>1E-4</v>
+        <v>0.01</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1">
@@ -2687,7 +4743,7 @@
       <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="6">
         <v>10</v>
       </c>
       <c r="L12" s="1">
@@ -2699,9 +4755,37 @@
       <c r="N12" s="1">
         <v>10</v>
       </c>
+      <c r="O12" s="1">
+        <v>10</v>
+      </c>
+      <c r="P12" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>10</v>
+      </c>
+      <c r="R12" s="1">
+        <v>10</v>
+      </c>
+      <c r="S12" s="1">
+        <v>10</v>
+      </c>
+      <c r="T12" s="1">
+        <v>10</v>
+      </c>
+      <c r="U12" s="1">
+        <v>10</v>
+      </c>
+      <c r="V12" s="1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K13" s="6"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1">
@@ -2731,7 +4815,7 @@
       <c r="J14" s="1">
         <v>0.96</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="6">
         <v>0.98</v>
       </c>
       <c r="L14" s="1">
@@ -2743,9 +4827,27 @@
       <c r="N14" s="1">
         <v>0.98</v>
       </c>
+      <c r="O14" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0.96</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1">
@@ -2775,7 +4877,7 @@
       <c r="J15" s="1">
         <v>0</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="6">
         <v>0.81</v>
       </c>
       <c r="L15" s="1">
@@ -2787,9 +4889,27 @@
       <c r="N15" s="1">
         <v>0.77</v>
       </c>
+      <c r="O15" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>0.77</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1">
@@ -2819,7 +4939,7 @@
       <c r="J16" s="1">
         <v>0.96</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="6">
         <v>0.98</v>
       </c>
       <c r="L16" s="1">
@@ -2831,9 +4951,27 @@
       <c r="N16" s="1">
         <v>0.98</v>
       </c>
+      <c r="O16" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0.96</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2863,7 +5001,7 @@
       <c r="J17" s="1">
         <v>0.22</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -2875,9 +5013,27 @@
       <c r="N17" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="O17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0.12</v>
+      </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1">
@@ -2907,7 +5063,7 @@
       <c r="J18" s="1">
         <v>0.85</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="6">
         <v>0.89</v>
       </c>
       <c r="L18" s="1">
@@ -2919,9 +5075,27 @@
       <c r="N18" s="1">
         <v>0.89</v>
       </c>
+      <c r="O18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0.9</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="1">
@@ -2943,7 +5117,7 @@
         <v>17.149999999999999</v>
       </c>
       <c r="H19" s="1">
-        <v>4.17</v>
+        <v>3.54</v>
       </c>
       <c r="I19" s="1">
         <v>4.34</v>
@@ -2951,74 +5125,128 @@
       <c r="J19" s="1">
         <v>4.33</v>
       </c>
-      <c r="K19" s="1">
-        <v>3.28</v>
+      <c r="K19" s="6">
+        <v>2.63</v>
       </c>
       <c r="L19" s="1">
-        <v>3.19</v>
+        <v>2.64</v>
       </c>
       <c r="M19" s="1">
         <v>3.46</v>
       </c>
       <c r="N19" s="1">
-        <v>4.0999999999999996</v>
+        <v>3.08</v>
+      </c>
+      <c r="O19" s="1">
+        <v>3.03</v>
+      </c>
+      <c r="P19" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>2.75</v>
+      </c>
+      <c r="R19" s="1">
+        <v>2.78</v>
+      </c>
+      <c r="S19" s="1">
+        <v>2.73</v>
+      </c>
+      <c r="T19" s="1">
+        <v>6.31</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K20" s="6"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <f>B14/B19</f>
+        <f t="shared" ref="B21:M21" si="0">B14/B19</f>
         <v>8.8262910798122055E-2</v>
       </c>
       <c r="C21" s="1">
-        <f>C14/C19</f>
+        <f t="shared" si="0"/>
         <v>0.14615384615384613</v>
       </c>
       <c r="D21" s="1">
-        <f>D14/D19</f>
+        <f t="shared" si="0"/>
         <v>0.14691943127962087</v>
       </c>
       <c r="E21" s="1">
-        <f>E14/E19</f>
+        <f t="shared" si="0"/>
         <v>5.09915014164306E-2</v>
       </c>
       <c r="F21" s="1">
-        <f>F14/F19</f>
+        <f t="shared" si="0"/>
         <v>5.3561253561253554E-2</v>
       </c>
       <c r="G21" s="1">
-        <f>G14/G19</f>
+        <f t="shared" si="0"/>
         <v>5.1311953352769682E-2</v>
       </c>
       <c r="H21" s="1">
-        <f>H14/H19</f>
-        <v>0.23261390887290168</v>
+        <f t="shared" si="0"/>
+        <v>0.27401129943502822</v>
       </c>
       <c r="I21" s="1">
-        <f>I14/I19</f>
+        <f t="shared" si="0"/>
         <v>0.22119815668202764</v>
       </c>
       <c r="J21" s="1">
-        <f>J14/J19</f>
+        <f t="shared" si="0"/>
         <v>0.22170900692840645</v>
       </c>
-      <c r="K21" s="1">
-        <f>K14/K19</f>
-        <v>0.29878048780487804</v>
+      <c r="K21" s="6">
+        <f t="shared" si="0"/>
+        <v>0.37262357414448671</v>
       </c>
       <c r="L21" s="1">
-        <f>L14/L19</f>
-        <v>0.30407523510971785</v>
+        <f t="shared" si="0"/>
+        <v>0.36742424242424238</v>
       </c>
       <c r="M21" s="1">
-        <f>M14/M19</f>
+        <f t="shared" si="0"/>
         <v>0.2774566473988439</v>
       </c>
       <c r="N21" s="1">
         <f>N14/N19</f>
-        <v>0.23902439024390246</v>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="O21" s="1">
+        <f>O14/O19</f>
+        <v>0.31683168316831684</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" ref="P21:Q21" si="1">P14/P19</f>
+        <v>0.30312499999999998</v>
+      </c>
+      <c r="Q21" s="6">
+        <f>Q14/Q19</f>
+        <v>0.35636363636363638</v>
+      </c>
+      <c r="R21" s="1">
+        <f>R14/R19</f>
+        <v>0.34892086330935251</v>
+      </c>
+      <c r="S21" s="1">
+        <f>S14/S19</f>
+        <v>0.35531135531135533</v>
+      </c>
+      <c r="T21" s="1">
+        <f t="shared" ref="T21:V21" si="2">T14/T19</f>
+        <v>0.15213946117274169</v>
+      </c>
+      <c r="U21" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V21" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push after fine tuning
</commit_message>
<xml_diff>
--- a/Batch_Optimization.xlsx
+++ b/Batch_Optimization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derrick\Documents\GitHub\Masters_Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E141A2-F13F-4C91-818C-5DCD2169CF06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73697FC-3E4B-4CA2-8D3C-303B9930213F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12285" windowHeight="5130" activeTab="1" xr2:uid="{E305303A-8BBB-401C-B59B-0762E69B7640}"/>
   </bookViews>
@@ -163,10 +163,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,12 +196,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -202,11 +214,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,21 +264,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -614,7 +678,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>362</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>135256</xdr:rowOff>
+      <xdr:rowOff>125731</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -746,7 +810,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>3778005</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>135255</xdr:rowOff>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -878,7 +942,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>334</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>131445</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1010,7 +1074,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>3778620</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1142,7 +1206,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>3778094</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>5715</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1274,7 +1338,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>56388</xdr:rowOff>
+      <xdr:rowOff>46863</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1406,7 +1470,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>3778620</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>81915</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1538,7 +1602,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>3780553</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1670,7 +1734,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>1033</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>17146</xdr:rowOff>
+      <xdr:rowOff>7621</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1802,7 +1866,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>3781170</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>59056</xdr:rowOff>
+      <xdr:rowOff>49531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1934,7 +1998,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3778676</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>120015</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2066,7 +2130,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>3778648</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>135256</xdr:rowOff>
+      <xdr:rowOff>125731</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2154,7 +2218,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>3781170</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2330,7 +2394,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>3702050</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2462,7 +2526,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>3724275</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3191,13 +3255,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49489416-574D-473C-A336-82E57285D721}">
-  <dimension ref="A2:S21"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L75" sqref="L75"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3206,6 +3270,7 @@
     <col min="2" max="19" width="56.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
@@ -3235,7 +3300,7 @@
       <c r="J2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -3294,7 +3359,7 @@
       <c r="J3" s="1">
         <v>10</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="9">
         <v>10</v>
       </c>
       <c r="L3" s="1">
@@ -3353,7 +3418,7 @@
       <c r="J4" s="1">
         <v>0.1</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="9">
         <v>0.1</v>
       </c>
       <c r="L4" s="1">
@@ -3412,7 +3477,7 @@
       <c r="J5" s="1">
         <v>0.5</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="9">
         <v>0.5</v>
       </c>
       <c r="L5" s="1">
@@ -3471,7 +3536,7 @@
       <c r="J6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="10" t="s">
         <v>38</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -3530,7 +3595,7 @@
       <c r="J7" s="1">
         <v>0.5</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="9">
         <v>0.5</v>
       </c>
       <c r="L7" s="1">
@@ -3589,7 +3654,7 @@
       <c r="J8" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="9">
         <v>1E-3</v>
       </c>
       <c r="L8" s="1">
@@ -3648,7 +3713,7 @@
       <c r="J9" s="1">
         <v>1000</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="9">
         <v>1000</v>
       </c>
       <c r="L9" s="1">
@@ -3676,121 +3741,121 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="6">
         <v>500</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="6">
         <v>500</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="6">
         <v>500</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="6">
         <v>100</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="6">
         <v>100</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="6">
         <v>100</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="6">
         <v>1000</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="6">
         <v>1000</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="6">
         <v>1000</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="11">
         <v>2000</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="6">
         <v>2000</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="6">
         <v>2000</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="6">
         <v>1500</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="6">
         <v>1500</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="6">
         <v>1250</v>
       </c>
       <c r="Q10" s="6">
         <v>1750</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="6">
         <v>1750</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" s="6">
         <v>1750</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="6">
         <v>0.01</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="6">
         <v>1E-4</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <v>0.01</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="6">
         <v>1E-4</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="6">
         <v>0.01</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="6">
         <v>1E-4</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="11">
         <v>0.1</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="6">
         <v>1E-4</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="6">
         <v>0.01</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="6">
         <v>0.01</v>
       </c>
       <c r="Q11" s="6">
         <v>0.01</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="6">
         <v>0.1</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="6">
         <v>1E-3</v>
       </c>
     </row>
@@ -3825,7 +3890,7 @@
       <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="9">
         <v>10</v>
       </c>
       <c r="L12" s="1">
@@ -3854,7 +3919,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K13" s="6"/>
+      <c r="K13" s="9"/>
       <c r="Q13" s="6"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -3864,7 +3929,7 @@
       <c r="B14" s="1">
         <v>0.98</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="9">
         <v>0.96</v>
       </c>
       <c r="Q14" s="6"/>
@@ -3876,7 +3941,7 @@
       <c r="B15" s="1">
         <v>0.84</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="9">
         <v>0</v>
       </c>
       <c r="Q15" s="6"/>
@@ -3888,7 +3953,7 @@
       <c r="B16" s="1">
         <v>0.98</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="9">
         <v>0.96</v>
       </c>
       <c r="Q16" s="6"/>
@@ -3900,7 +3965,7 @@
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="9">
         <v>0.12</v>
       </c>
       <c r="Q17" s="6"/>
@@ -3912,7 +3977,7 @@
       <c r="B18" s="1">
         <v>0.9</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="9">
         <v>0.89</v>
       </c>
       <c r="Q18" s="6"/>
@@ -3924,13 +3989,13 @@
       <c r="B19" s="1">
         <v>58.68</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="9">
         <v>35.26</v>
       </c>
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K20" s="6"/>
+      <c r="K20" s="9"/>
       <c r="Q20" s="6"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -3973,7 +4038,7 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="9">
         <f t="shared" si="0"/>
         <v>2.7226318774815655E-2</v>
       </c>
@@ -4009,6 +4074,150 @@
         <f>S14/S19</f>
         <v>#DIV/0!</v>
       </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K30" s="9"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K31" s="9"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="9"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="9"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="9"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="9"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="9"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="9"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="9"/>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="9"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="9"/>
+    </row>
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="9"/>
+    </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="9"/>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="9"/>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="9"/>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="9"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="9"/>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="9"/>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="9"/>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="9"/>
+    </row>
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="9"/>
+    </row>
+    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="9"/>
+    </row>
+    <row r="55" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="9"/>
+    </row>
+    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="9"/>
+    </row>
+    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="9"/>
+    </row>
+    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="9"/>
+    </row>
+    <row r="59" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K59" s="9"/>
+    </row>
+    <row r="60" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="9"/>
+    </row>
+    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="9"/>
+    </row>
+    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="9"/>
+    </row>
+    <row r="63" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K63" s="9"/>
+    </row>
+    <row r="64" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K64" s="9"/>
+    </row>
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="9"/>
+    </row>
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="9"/>
+    </row>
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="9"/>
+    </row>
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="9"/>
+    </row>
+    <row r="69" spans="11:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K69" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4019,21 +4228,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2357D04-C28B-44E3-B5FB-928058F75E94}">
-  <dimension ref="A2:V21"/>
+  <dimension ref="A1:V69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T20" sqref="T20"/>
+      <selection pane="bottomRight" activeCell="Q10" sqref="Q10:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="22" width="56.7109375" style="1" customWidth="1"/>
+    <col min="2" max="19" width="56.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
@@ -4063,7 +4273,7 @@
       <c r="J2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -4081,7 +4291,7 @@
       <c r="P2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="8" t="s">
         <v>35</v>
       </c>
       <c r="R2" s="4" t="s">
@@ -4090,13 +4300,13 @@
       <c r="S2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4131,7 +4341,7 @@
       <c r="J3" s="1">
         <v>10</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="9">
         <v>10</v>
       </c>
       <c r="L3" s="1">
@@ -4149,7 +4359,7 @@
       <c r="P3" s="1">
         <v>10</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="9">
         <v>10</v>
       </c>
       <c r="R3" s="1">
@@ -4158,13 +4368,13 @@
       <c r="S3" s="1">
         <v>10</v>
       </c>
-      <c r="T3" s="1">
-        <v>10</v>
-      </c>
-      <c r="U3" s="1">
-        <v>10</v>
-      </c>
-      <c r="V3" s="1">
+      <c r="T3">
+        <v>10</v>
+      </c>
+      <c r="U3">
+        <v>10</v>
+      </c>
+      <c r="V3">
         <v>10</v>
       </c>
     </row>
@@ -4199,7 +4409,7 @@
       <c r="J4" s="1">
         <v>0.1</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="9">
         <v>0.1</v>
       </c>
       <c r="L4" s="1">
@@ -4217,7 +4427,7 @@
       <c r="P4" s="1">
         <v>0.1</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="9">
         <v>0.1</v>
       </c>
       <c r="R4" s="1">
@@ -4226,13 +4436,13 @@
       <c r="S4" s="1">
         <v>0.1</v>
       </c>
-      <c r="T4" s="1">
+      <c r="T4">
         <v>0.1</v>
       </c>
-      <c r="U4" s="1">
+      <c r="U4">
         <v>0.1</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4">
         <v>0.1</v>
       </c>
     </row>
@@ -4267,7 +4477,7 @@
       <c r="J5" s="1">
         <v>0.5</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="9">
         <v>0.5</v>
       </c>
       <c r="L5" s="1">
@@ -4285,7 +4495,7 @@
       <c r="P5" s="1">
         <v>0.5</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="9">
         <v>0.5</v>
       </c>
       <c r="R5" s="1">
@@ -4294,13 +4504,13 @@
       <c r="S5" s="1">
         <v>0.5</v>
       </c>
-      <c r="T5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="V5" s="1">
+      <c r="T5">
+        <v>0.5</v>
+      </c>
+      <c r="U5">
+        <v>0.5</v>
+      </c>
+      <c r="V5">
         <v>0.5</v>
       </c>
     </row>
@@ -4335,7 +4545,7 @@
       <c r="J6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -4353,7 +4563,7 @@
       <c r="P6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="Q6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -4362,13 +4572,13 @@
       <c r="S6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" t="s">
         <v>18</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="U6" t="s">
         <v>18</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="V6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4403,7 +4613,7 @@
       <c r="J7" s="1">
         <v>0.5</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="9">
         <v>0.5</v>
       </c>
       <c r="L7" s="1">
@@ -4421,7 +4631,7 @@
       <c r="P7" s="1">
         <v>0.5</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="9">
         <v>0.5</v>
       </c>
       <c r="R7" s="1">
@@ -4430,13 +4640,13 @@
       <c r="S7" s="1">
         <v>0.5</v>
       </c>
-      <c r="T7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="U7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="V7" s="1">
+      <c r="T7">
+        <v>0.5</v>
+      </c>
+      <c r="U7">
+        <v>0.5</v>
+      </c>
+      <c r="V7">
         <v>0.5</v>
       </c>
     </row>
@@ -4471,7 +4681,7 @@
       <c r="J8" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="9">
         <v>1E-3</v>
       </c>
       <c r="L8" s="1">
@@ -4489,7 +4699,7 @@
       <c r="P8" s="1">
         <v>1E-3</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="9">
         <v>1E-3</v>
       </c>
       <c r="R8" s="1">
@@ -4498,13 +4708,13 @@
       <c r="S8" s="1">
         <v>1E-3</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8">
         <v>1E-3</v>
       </c>
-      <c r="U8" s="1">
+      <c r="U8">
         <v>1E-3</v>
       </c>
-      <c r="V8" s="1">
+      <c r="V8">
         <v>1E-3</v>
       </c>
     </row>
@@ -4539,7 +4749,7 @@
       <c r="J9" s="1">
         <v>1000</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="9">
         <v>1000</v>
       </c>
       <c r="L9" s="1">
@@ -4557,7 +4767,7 @@
       <c r="P9" s="1">
         <v>1000</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="9">
         <v>1000</v>
       </c>
       <c r="R9" s="1">
@@ -4566,149 +4776,149 @@
       <c r="S9" s="1">
         <v>1000</v>
       </c>
-      <c r="T9" s="1">
+      <c r="T9">
         <v>3000</v>
       </c>
-      <c r="U9" s="1">
+      <c r="U9">
         <v>1000</v>
       </c>
-      <c r="V9" s="1">
+      <c r="V9">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="6">
         <v>500</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="6">
         <v>500</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="6">
         <v>500</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="6">
         <v>100</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="6">
         <v>100</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="6">
         <v>100</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="6">
         <v>1000</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="6">
         <v>1000</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="6">
         <v>1000</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="11">
         <v>2000</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="6">
         <v>2000</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="6">
         <v>2000</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="6">
         <v>1500</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="6">
         <v>1500</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="6">
         <v>1250</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="11">
         <v>1750</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="6">
         <v>1750</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" s="6">
         <v>1750</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10" s="7">
         <v>2000</v>
       </c>
-      <c r="U10" s="1">
+      <c r="U10" s="7">
         <v>2000</v>
       </c>
-      <c r="V10" s="1">
+      <c r="V10" s="7">
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="6">
         <v>0.01</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="6">
         <v>1E-4</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <v>0.01</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="6">
         <v>1E-4</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="6">
         <v>0.01</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="6">
         <v>1E-4</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="11">
         <v>0.01</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="6">
         <v>1E-4</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="6">
         <v>0.01</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="6">
         <v>0.01</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="11">
         <v>0.01</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="6">
         <v>0.1</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="6">
         <v>1E-3</v>
       </c>
-      <c r="T11" s="1">
+      <c r="T11" s="7">
         <v>0.1</v>
       </c>
-      <c r="U11" s="1">
+      <c r="U11" s="7">
         <v>0.01</v>
       </c>
-      <c r="V11" s="1">
+      <c r="V11" s="7">
         <v>1E-3</v>
       </c>
     </row>
@@ -4743,7 +4953,7 @@
       <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="9">
         <v>10</v>
       </c>
       <c r="L12" s="1">
@@ -4761,7 +4971,7 @@
       <c r="P12" s="1">
         <v>10</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="9">
         <v>10</v>
       </c>
       <c r="R12" s="1">
@@ -4770,19 +4980,19 @@
       <c r="S12" s="1">
         <v>10</v>
       </c>
-      <c r="T12" s="1">
-        <v>10</v>
-      </c>
-      <c r="U12" s="1">
-        <v>10</v>
-      </c>
-      <c r="V12" s="1">
+      <c r="T12">
+        <v>10</v>
+      </c>
+      <c r="U12">
+        <v>10</v>
+      </c>
+      <c r="V12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K13" s="6"/>
-      <c r="Q13" s="6"/>
+      <c r="K13" s="9"/>
+      <c r="Q13" s="9"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -4815,7 +5025,7 @@
       <c r="J14" s="1">
         <v>0.96</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="9">
         <v>0.98</v>
       </c>
       <c r="L14" s="1">
@@ -4833,7 +5043,7 @@
       <c r="P14" s="1">
         <v>0.97</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14" s="9">
         <v>0.98</v>
       </c>
       <c r="R14" s="1">
@@ -4842,7 +5052,7 @@
       <c r="S14" s="1">
         <v>0.97</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14">
         <v>0.96</v>
       </c>
     </row>
@@ -4877,7 +5087,7 @@
       <c r="J15" s="1">
         <v>0</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="9">
         <v>0.81</v>
       </c>
       <c r="L15" s="1">
@@ -4895,7 +5105,7 @@
       <c r="P15" s="1">
         <v>0.65</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="Q15" s="9">
         <v>0.77</v>
       </c>
       <c r="R15" s="1">
@@ -4904,7 +5114,7 @@
       <c r="S15" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="T15" s="1">
+      <c r="T15">
         <v>0.1</v>
       </c>
     </row>
@@ -4939,7 +5149,7 @@
       <c r="J16" s="1">
         <v>0.96</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="9">
         <v>0.98</v>
       </c>
       <c r="L16" s="1">
@@ -4957,7 +5167,7 @@
       <c r="P16" s="1">
         <v>0.97</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="Q16" s="9">
         <v>0.98</v>
       </c>
       <c r="R16" s="1">
@@ -4966,7 +5176,7 @@
       <c r="S16" s="1">
         <v>0.97</v>
       </c>
-      <c r="T16" s="1">
+      <c r="T16">
         <v>0.96</v>
       </c>
     </row>
@@ -5001,7 +5211,7 @@
       <c r="J17" s="1">
         <v>0.22</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="K17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -5019,7 +5229,7 @@
       <c r="P17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q17" s="6" t="s">
+      <c r="Q17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="R17" s="1" t="s">
@@ -5028,7 +5238,7 @@
       <c r="S17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T17" s="1">
+      <c r="T17">
         <v>0.12</v>
       </c>
     </row>
@@ -5063,7 +5273,7 @@
       <c r="J18" s="1">
         <v>0.85</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="9">
         <v>0.89</v>
       </c>
       <c r="L18" s="1">
@@ -5081,7 +5291,7 @@
       <c r="P18" s="1">
         <v>0.88</v>
       </c>
-      <c r="Q18" s="6">
+      <c r="Q18" s="9">
         <v>0.89</v>
       </c>
       <c r="R18" s="1">
@@ -5090,7 +5300,7 @@
       <c r="S18" s="1">
         <v>0.9</v>
       </c>
-      <c r="T18" s="1">
+      <c r="T18">
         <v>0.9</v>
       </c>
     </row>
@@ -5125,7 +5335,7 @@
       <c r="J19" s="1">
         <v>4.33</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="9">
         <v>2.63</v>
       </c>
       <c r="L19" s="1">
@@ -5143,7 +5353,7 @@
       <c r="P19" s="1">
         <v>3.2</v>
       </c>
-      <c r="Q19" s="6">
+      <c r="Q19" s="9">
         <v>2.75</v>
       </c>
       <c r="R19" s="1">
@@ -5152,13 +5362,13 @@
       <c r="S19" s="1">
         <v>2.73</v>
       </c>
-      <c r="T19" s="1">
+      <c r="T19">
         <v>6.31</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K20" s="6"/>
-      <c r="Q20" s="6"/>
+      <c r="K20" s="9"/>
+      <c r="Q20" s="9"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -5200,7 +5410,7 @@
         <f t="shared" si="0"/>
         <v>0.22170900692840645</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="9">
         <f t="shared" si="0"/>
         <v>0.37262357414448671</v>
       </c>
@@ -5224,7 +5434,7 @@
         <f t="shared" ref="P21:Q21" si="1">P14/P19</f>
         <v>0.30312499999999998</v>
       </c>
-      <c r="Q21" s="6">
+      <c r="Q21" s="9">
         <f>Q14/Q19</f>
         <v>0.35636363636363638</v>
       </c>
@@ -5236,18 +5446,209 @@
         <f>S14/S19</f>
         <v>0.35531135531135533</v>
       </c>
-      <c r="T21" s="1">
+      <c r="T21">
         <f t="shared" ref="T21:V21" si="2">T14/T19</f>
         <v>0.15213946117274169</v>
       </c>
-      <c r="U21" s="1" t="e">
+      <c r="U21" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="V21" s="1" t="e">
+      <c r="V21" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K22" s="9"/>
+      <c r="Q22" s="9"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K23" s="9"/>
+      <c r="Q23" s="9"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K24" s="9"/>
+      <c r="Q24" s="9"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K25" s="9"/>
+      <c r="Q25" s="9"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K26" s="9"/>
+      <c r="Q26" s="9"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K27" s="9"/>
+      <c r="Q27" s="9"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K28" s="9"/>
+      <c r="Q28" s="9"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K29" s="9"/>
+      <c r="Q29" s="9"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K30" s="9"/>
+      <c r="Q30" s="9"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K31" s="9"/>
+      <c r="Q31" s="9"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K32" s="9"/>
+      <c r="Q32" s="9"/>
+    </row>
+    <row r="33" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K33" s="9"/>
+      <c r="Q33" s="9"/>
+    </row>
+    <row r="34" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K34" s="9"/>
+      <c r="Q34" s="9"/>
+    </row>
+    <row r="35" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K35" s="9"/>
+      <c r="Q35" s="9"/>
+    </row>
+    <row r="36" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K36" s="9"/>
+      <c r="Q36" s="9"/>
+    </row>
+    <row r="37" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K37" s="9"/>
+      <c r="Q37" s="9"/>
+    </row>
+    <row r="38" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K38" s="9"/>
+      <c r="Q38" s="9"/>
+    </row>
+    <row r="39" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K39" s="9"/>
+      <c r="Q39" s="9"/>
+    </row>
+    <row r="40" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K40" s="9"/>
+      <c r="Q40" s="9"/>
+    </row>
+    <row r="41" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K41" s="9"/>
+      <c r="Q41" s="9"/>
+    </row>
+    <row r="42" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K42" s="9"/>
+      <c r="Q42" s="9"/>
+    </row>
+    <row r="43" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K43" s="9"/>
+      <c r="Q43" s="9"/>
+    </row>
+    <row r="44" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K44" s="9"/>
+      <c r="Q44" s="9"/>
+    </row>
+    <row r="45" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K45" s="9"/>
+      <c r="Q45" s="9"/>
+    </row>
+    <row r="46" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K46" s="9"/>
+      <c r="Q46" s="9"/>
+    </row>
+    <row r="47" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K47" s="9"/>
+      <c r="Q47" s="9"/>
+    </row>
+    <row r="48" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K48" s="9"/>
+      <c r="Q48" s="9"/>
+    </row>
+    <row r="49" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K49" s="9"/>
+      <c r="Q49" s="9"/>
+    </row>
+    <row r="50" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K50" s="9"/>
+      <c r="Q50" s="9"/>
+    </row>
+    <row r="51" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K51" s="9"/>
+      <c r="Q51" s="9"/>
+    </row>
+    <row r="52" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K52" s="9"/>
+      <c r="Q52" s="9"/>
+    </row>
+    <row r="53" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K53" s="9"/>
+      <c r="Q53" s="9"/>
+    </row>
+    <row r="54" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K54" s="9"/>
+      <c r="Q54" s="9"/>
+    </row>
+    <row r="55" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K55" s="9"/>
+      <c r="Q55" s="9"/>
+    </row>
+    <row r="56" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K56" s="9"/>
+      <c r="Q56" s="9"/>
+    </row>
+    <row r="57" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K57" s="9"/>
+      <c r="Q57" s="9"/>
+    </row>
+    <row r="58" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K58" s="9"/>
+      <c r="Q58" s="9"/>
+    </row>
+    <row r="59" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K59" s="9"/>
+      <c r="Q59" s="9"/>
+    </row>
+    <row r="60" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K60" s="9"/>
+      <c r="Q60" s="9"/>
+    </row>
+    <row r="61" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K61" s="9"/>
+      <c r="Q61" s="9"/>
+    </row>
+    <row r="62" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K62" s="9"/>
+      <c r="Q62" s="9"/>
+    </row>
+    <row r="63" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K63" s="9"/>
+      <c r="Q63" s="9"/>
+    </row>
+    <row r="64" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K64" s="9"/>
+      <c r="Q64" s="9"/>
+    </row>
+    <row r="65" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K65" s="9"/>
+      <c r="Q65" s="9"/>
+    </row>
+    <row r="66" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K66" s="9"/>
+      <c r="Q66" s="9"/>
+    </row>
+    <row r="67" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K67" s="9"/>
+      <c r="Q67" s="9"/>
+    </row>
+    <row r="68" spans="11:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K68" s="9"/>
+      <c r="Q68" s="12"/>
+    </row>
+    <row r="69" spans="11:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K69" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>